<commit_message>
Se optimizo el codigo
</commit_message>
<xml_diff>
--- a/MATERIAS-1.xlsx
+++ b/MATERIAS-1.xlsx
@@ -5,22 +5,25 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOPORTE\Desktop\Whatsapp_bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOPORTE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068F242C-064F-4B54-B83F-C36698F1ABF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE5DC3C-59DF-4E4E-A4B6-3B94679C9CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="4" xr2:uid="{EE5CF061-FBF5-4F11-96CE-FF5E0DDB9EE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1 (4)" sheetId="2" r:id="rId2"/>
-    <sheet name="si" sheetId="3" r:id="rId3"/>
-    <sheet name="Hoja1 (3)" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1 (4)" sheetId="4" r:id="rId2"/>
+    <sheet name="si" sheetId="2" r:id="rId3"/>
+    <sheet name="Hoja1 (3)" sheetId="3" r:id="rId4"/>
     <sheet name="final" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -33,7 +36,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="124">
+  <si>
+    <t>DISEÑO DE COMPILADORES</t>
+  </si>
+  <si>
+    <t>PROYECTO INTEGRADOR DE DESARROLLO DE SOLUCIONES EMPRESARIALES</t>
+  </si>
+  <si>
+    <t>TALLER DE GRADUACION</t>
+  </si>
   <si>
     <t>Nombre materia</t>
   </si>
@@ -47,27 +59,18 @@
     <t>gestion</t>
   </si>
   <si>
-    <t>DISEÑO DE COMPILADORES</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>1/2022</t>
   </si>
   <si>
-    <t>PROYECTO INTEGRADOR DE DESARROLLO DE SOLUCIONES EMPRESARIALES</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>TALLER DE GRADUACION</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Nombre</t>
   </si>
   <si>
@@ -101,157 +104,298 @@
     <t>GRADUACION</t>
   </si>
   <si>
+    <t>MATEMÁTICAS</t>
+  </si>
+  <si>
+    <t>DISCRETAS</t>
+  </si>
+  <si>
+    <t>FUNDAMENTOS</t>
+  </si>
+  <si>
+    <t>CIENCIA</t>
+  </si>
+  <si>
+    <t>COMPUTACION</t>
+  </si>
+  <si>
+    <t>ADMINISTRACION</t>
+  </si>
+  <si>
+    <t>PROGRAMACION</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>DATOS</t>
+  </si>
+  <si>
+    <t>INTRODUCCIÓN</t>
+  </si>
+  <si>
+    <t>INFORMÁTICA</t>
+  </si>
+  <si>
+    <t>INFORMATICA</t>
+  </si>
+  <si>
+    <t>APLICADA</t>
+  </si>
+  <si>
+    <t>PROGRAMACIÓN</t>
+  </si>
+  <si>
+    <t>LÓGICA</t>
+  </si>
+  <si>
+    <t>FUNCIONAL</t>
+  </si>
+  <si>
+    <t>ORGANIZACIÓN</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA</t>
+  </si>
+  <si>
+    <t>COMPUTADORAS</t>
+  </si>
+  <si>
+    <t>ADMINISTRACIÓN</t>
+  </si>
+  <si>
+    <t>SISTEMAS</t>
+  </si>
+  <si>
+    <t>OPERATIVOS</t>
+  </si>
+  <si>
+    <t>INFRAESTRUCTURA</t>
+  </si>
+  <si>
+    <t>TI</t>
+  </si>
+  <si>
+    <t>TECNOLOGÍAS</t>
+  </si>
+  <si>
+    <t>EMERGENTES</t>
+  </si>
+  <si>
+    <t>COMUNICACION</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>COMUNICACIÓN</t>
+  </si>
+  <si>
+    <t>TEORIA</t>
+  </si>
+  <si>
+    <t>COMUNICACIONES</t>
+  </si>
+  <si>
+    <t>EMPRESARIAL</t>
+  </si>
+  <si>
+    <t>ANTENAS</t>
+  </si>
+  <si>
+    <t>RADIO</t>
+  </si>
+  <si>
+    <t>REDES</t>
+  </si>
+  <si>
+    <t>CABLEADO</t>
+  </si>
+  <si>
+    <t>ESTRUCTURADO</t>
+  </si>
+  <si>
+    <t>INSTALACION</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>APLICACIONES</t>
+  </si>
+  <si>
+    <t>COMPUTACIÓN</t>
+  </si>
+  <si>
+    <t>PARALELA</t>
+  </si>
+  <si>
+    <t>DISTRIBUIDA</t>
+  </si>
+  <si>
     <t>abreviacion</t>
   </si>
   <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>2M</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>TU</t>
+  </si>
+  <si>
+    <t>MATE DISC   Grp.W1</t>
+  </si>
+  <si>
+    <t>FUND CIEN COM  Grp.M</t>
+  </si>
+  <si>
+    <t>ADMI PROG BAS DAT Grp.C</t>
+  </si>
+  <si>
+    <t>INTR INFO   Grp.1M</t>
+  </si>
+  <si>
+    <t>PROG LÓGI FUN  Grp.A</t>
+  </si>
+  <si>
+    <t>PROY INTE DES SOL Grp.S1</t>
+  </si>
+  <si>
+    <t>INTR INFO   Grp.2M</t>
+  </si>
+  <si>
+    <t>ORGA ARQU COM  Grp.A</t>
+  </si>
+  <si>
+    <t>ADMI SIST OPE  Grp.A</t>
+  </si>
+  <si>
+    <t>INFR TI TEC EME Grp.S1</t>
+  </si>
+  <si>
+    <t>COMU I   Grp.A</t>
+  </si>
+  <si>
+    <t>FUND COMU   Grp.A</t>
+  </si>
+  <si>
+    <t>TEOR COMU   Grp.C</t>
+  </si>
+  <si>
+    <t>INTR INFO   Grp.F</t>
+  </si>
+  <si>
+    <t>PROY EMPR   Grp.11</t>
+  </si>
+  <si>
+    <t>MATE DISC   Grp.L</t>
+  </si>
+  <si>
+    <t>FUND CIEN COM  Grp.J</t>
+  </si>
+  <si>
+    <t>TALL PROG   Grp.B</t>
+  </si>
+  <si>
+    <t>ORGA ARQU COM  Grp.S1</t>
+  </si>
+  <si>
+    <t>ADMI SIST OPE  Grp.SN</t>
+  </si>
+  <si>
+    <t>INFR TI TEC EME Grp.SN</t>
+  </si>
+  <si>
+    <t>ANTE SIST RAD  Grp.R1</t>
+  </si>
+  <si>
+    <t>TALL REDE   Grp.RN</t>
+  </si>
+  <si>
+    <t>DISE CABL EST  Grp.R2</t>
+  </si>
+  <si>
+    <t>CABL ESTR   Grp.RN</t>
+  </si>
+  <si>
+    <t>INST REDE   Grp.H</t>
+  </si>
+  <si>
+    <t>PROG III   Grp.TU</t>
+  </si>
+  <si>
+    <t>ADMI SIST OPE VI Grp.TU</t>
+  </si>
+  <si>
+    <t>DESA APLI VI  Grp.TU</t>
+  </si>
+  <si>
+    <t>COMP PARA DIS  Grp.TU</t>
+  </si>
+  <si>
     <t>abreviacion-texto</t>
   </si>
   <si>
-    <t>MATEMÁTICAS</t>
-  </si>
-  <si>
-    <t>DISCRETAS</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>W1</t>
-  </si>
-  <si>
-    <t>FUNDAMENTOS</t>
-  </si>
-  <si>
-    <t>CIENCIA</t>
-  </si>
-  <si>
-    <t>COMPUTACION</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>M1</t>
-  </si>
-  <si>
-    <t>ADMINISTRACION</t>
-  </si>
-  <si>
-    <t>PROGRAMACION</t>
-  </si>
-  <si>
-    <t>BASE</t>
-  </si>
-  <si>
-    <t>DATOS</t>
-  </si>
-  <si>
-    <t>INTRODUCCIÓN</t>
-  </si>
-  <si>
-    <t>INFORMÁTICA</t>
-  </si>
-  <si>
-    <t>1M</t>
-  </si>
-  <si>
-    <t>INFORMATICA</t>
-  </si>
-  <si>
-    <t>APLICADA</t>
-  </si>
-  <si>
     <t>TEC</t>
   </si>
   <si>
-    <t>PROGRAMACIÓN</t>
-  </si>
-  <si>
-    <t>LÓGICA</t>
-  </si>
-  <si>
-    <t>FUNCIONAL</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>2M</t>
-  </si>
-  <si>
-    <t>INTR INFO   Grp.2M</t>
-  </si>
-  <si>
-    <t>F</t>
+    <t>INFO APLI TEC  Grp.C</t>
   </si>
   <si>
     <t>INFO APLI TEC  Grp.F</t>
   </si>
   <si>
-    <t>ORGANIZACIÓN</t>
-  </si>
-  <si>
-    <t>ARQUITECTURA</t>
-  </si>
-  <si>
-    <t>COMPUTADORAS</t>
-  </si>
-  <si>
-    <t>ORGA ARQU COM  Grp.A</t>
-  </si>
-  <si>
-    <t>ADMINISTRACIÓN</t>
-  </si>
-  <si>
-    <t>SISTEMAS</t>
-  </si>
-  <si>
-    <t>OPERATIVOS</t>
-  </si>
-  <si>
-    <t>ADMI SIST OPE  Grp.A</t>
-  </si>
-  <si>
-    <t>INFRAESTRUCTURA</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>TECNOLOGÍAS</t>
-  </si>
-  <si>
-    <t>EMERGENTES</t>
-  </si>
-  <si>
-    <t>INFR TI TEC EME Grp.S1</t>
-  </si>
-  <si>
-    <t>COMUNICACION</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>COMU I   Grp.A</t>
-  </si>
-  <si>
-    <t>COMUNICACIÓN</t>
-  </si>
-  <si>
-    <t>FUND COMU   Grp.A</t>
-  </si>
-  <si>
-    <t>TEORIA</t>
-  </si>
-  <si>
-    <t>COMUNICACIONES</t>
-  </si>
-  <si>
-    <t>TEOR COMU   Grp.C</t>
-  </si>
-  <si>
-    <t>INTR INFO   Grp.F</t>
+    <t>INFO APLI TEC  Grp.E</t>
   </si>
   <si>
     <t>SEMI</t>
@@ -260,134 +404,17 @@
     <t>INTR INFO SEM  Grp.B</t>
   </si>
   <si>
-    <t>EMPRESARIAL</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>PROY EMPR   Grp.11</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>MATE DISC   Grp.L</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
-    <t>FUND CIEN COM  Grp.J</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>INFO APLI TEC  Grp.E</t>
-  </si>
-  <si>
-    <t>TALL PROG   Grp.B</t>
-  </si>
-  <si>
-    <t>ORGA ARQU COM  Grp.S1</t>
-  </si>
-  <si>
-    <t>SN</t>
-  </si>
-  <si>
-    <t>ADMI SIST OPE  Grp.SN</t>
-  </si>
-  <si>
-    <t>INFR TI TEC EME Grp.SN</t>
-  </si>
-  <si>
-    <t>ANTENAS</t>
-  </si>
-  <si>
-    <t>RADIO</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>ANTE SIST RAD  Grp.R1</t>
-  </si>
-  <si>
-    <t>REDES</t>
-  </si>
-  <si>
-    <t>RN</t>
-  </si>
-  <si>
-    <t>TALL REDE   Grp.RN</t>
-  </si>
-  <si>
-    <t>CABLEADO</t>
-  </si>
-  <si>
-    <t>ESTRUCTURADO</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>DISE CABL EST  Grp.R2</t>
-  </si>
-  <si>
-    <t>CABL ESTR   Grp.RN</t>
-  </si>
-  <si>
-    <t>INSTALACION</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>INST REDE   Grp.H</t>
-  </si>
-  <si>
     <t>INTR INFO SEM  Grp.C</t>
   </si>
   <si>
-    <t>III</t>
-  </si>
-  <si>
-    <t>TU</t>
-  </si>
-  <si>
-    <t>PROG III   Grp.TU</t>
-  </si>
-  <si>
-    <t>VI</t>
-  </si>
-  <si>
-    <t>ADMI SIST OPE VI Grp.TU</t>
-  </si>
-  <si>
-    <t>APLICACIONES</t>
-  </si>
-  <si>
-    <t>DESA APLI VI  Grp.TU</t>
-  </si>
-  <si>
-    <t>COMPUTACIÓN</t>
-  </si>
-  <si>
-    <t>PARALELA</t>
-  </si>
-  <si>
-    <t>DISTRIBUIDA</t>
-  </si>
-  <si>
-    <t>COMP PARA DIS  Grp.TU</t>
+    <t>INICIO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,6 +437,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -425,7 +466,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -448,38 +489,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -490,9 +510,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -514,17 +531,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -838,7 +848,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2220C26-586D-4009-B007-7E292AF50089}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -848,36 +858,36 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="64" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" style="2"/>
     <col min="5" max="5" width="42.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" t="str">
         <f>A2&amp;" Grp."&amp;B2&amp;" Mod."&amp;C2&amp;" - "&amp;D2</f>
@@ -886,7 +896,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -895,35 +905,35 @@
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3" t="str">
         <f>MID(A3,1,3)&amp;" Grp."&amp;B2&amp;" Mod."&amp;C2&amp;" - "&amp;D2</f>
         <v>PRO Grp.A Mod.1 - 1/2022</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67350636-05DA-4E50-8501-74C8C625FBB6}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -932,14 +942,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.5546875" style="5"/>
     <col min="11" max="11" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -947,40 +957,40 @@
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>6</v>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(MID(A2,1,4),".",MID(B2,1,4),".",MID(C2,1,4)," Grp.",H2," Mod.",I2," Grp.",J2)</f>
@@ -988,59 +998,59 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>6</v>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K3" t="str">
         <f>CONCATENATE(MID(A3,1,3),".",MID(B3,1,3),".",MID(C3,1,3),".",MID(D3,1,3),".",MID(E3,1,3),".",MID(F3,1,3),".",MID(G3,1,3)," Grp.",H3," Mod.",I3," Grp.",J3)</f>
         <v>PRO.INT.DE.DES.DE.SOL.EMP Grp.B Mod.1 Grp.1/2022</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>6</v>
+      <c r="H4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE(MID(A4,1,4)," ",MID(B4,1,4)," ",MID(C4,1,4)," ",MID(D4,1,4)," Grp.",H4," Mod.",I4," ",J4)</f>
@@ -1052,12 +1062,12 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{182DA3A7-9107-4A4F-9EAC-15CA4C8847B4}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1066,14 +1076,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="11.5546875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="11.5546875" style="5"/>
     <col min="11" max="11" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1081,40 +1091,40 @@
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>3</v>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="4">
-        <v>1</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>6</v>
+      <c r="H2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE(MID(A2,1,4),".",MID(B2,1,4),".",MID(C2,1,4)," Grp.",H2," Mod.",I2," Grp.",J2)</f>
@@ -1122,59 +1132,59 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="4">
-        <v>1</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>6</v>
+      <c r="I3" s="5">
+        <v>1</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K3" t="str">
         <f>CONCATENATE(MID(A3,1,3),".",MID(B3,1,3),".",MID(C3,1,3),".",MID(D3,1,3),".",MID(E3,1,3),".",MID(F3,1,3),".",MID(G3,1,3)," Grp.",H3," Mod.",I3," Grp.",J3)</f>
         <v>PRO.INT.DE.DES.DE.SOL.EMP Grp.B Mod.1 Grp.1/2022</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="4">
-        <v>1</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>6</v>
+      <c r="H4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5">
+        <v>1</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE(MID(A4,1,4)," ",MID(B4,1,4)," ",MID(C4,1,4)," ",MID(D4,1,4)," Grp.",H4," Mod.",I4," ",J4)</f>
@@ -1182,16 +1192,17 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52A9271-DF39-4B9E-BB79-64A1274B2916}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1204,13 +1215,13 @@
     <col min="2" max="2" width="1.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.21875" customWidth="1"/>
     <col min="4" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" style="2"/>
     <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -1234,18 +1245,18 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <f>SEARCH(" ",A2,1)</f>
@@ -1276,45 +1287,45 @@
         <v>#VALUE!</v>
       </c>
       <c r="I2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <f>SEARCH(" ",A3,1)</f>
+        <f t="shared" ref="B3:B4" si="0">SEARCH(" ",A3,1)</f>
         <v>9</v>
       </c>
       <c r="C3">
-        <f>SEARCH(" ",A3,B3+1)</f>
+        <f t="shared" ref="C3:C4" si="1">SEARCH(" ",A3,B3+1)</f>
         <v>20</v>
       </c>
       <c r="D3">
-        <f>SEARCH(" ",A3,C3+1)</f>
+        <f t="shared" ref="D3:D4" si="2">SEARCH(" ",A3,C3+1)</f>
         <v>23</v>
       </c>
       <c r="E3">
-        <f>SEARCH(" ",A3,D3+1)</f>
+        <f t="shared" ref="E3:E4" si="3">SEARCH(" ",A3,D3+1)</f>
         <v>34</v>
       </c>
       <c r="F3">
-        <f>SEARCH(" ",A3,E3+1)</f>
+        <f t="shared" ref="F3:F4" si="4">SEARCH(" ",A3,E3+1)</f>
         <v>37</v>
       </c>
       <c r="G3">
-        <f>SEARCH(" ",A3,F3+1)</f>
+        <f t="shared" ref="G3:G4" si="5">SEARCH(" ",A3,F3+1)</f>
         <v>48</v>
       </c>
       <c r="H3" t="e">
-        <f>SEARCH(" ",A3,G3+1)</f>
+        <f t="shared" ref="H3:H4" si="6">SEARCH(" ",A3,G3+1)</f>
         <v>#VALUE!</v>
       </c>
       <c r="I3" t="s">
@@ -1324,187 +1335,186 @@
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E4" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F4" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <f>SEARCH(" ",A4,1)</f>
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <f>SEARCH(" ",A4,B4+1)</f>
-        <v>10</v>
-      </c>
-      <c r="D4" t="e">
-        <f>SEARCH(" ",A4,C4+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E4" t="e">
-        <f>SEARCH(" ",A4,D4+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F4" t="e">
-        <f>SEARCH(" ",A4,E4+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G4" t="e">
-        <f>SEARCH(" ",A4,F4+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H4" t="e">
-        <f>SEARCH(" ",A4,G4+1)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I4" t="s">
-        <v>10</v>
-      </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D70149-973D-4F71-961A-D236D5FCE0B9}">
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
       <c r="F1" s="11" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="J1" s="12" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>25</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="9"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I2" s="13" t="str">
-        <f t="shared" ref="I2:I39" si="0">CONCATENATE(MID(A2,1,4)," ",MID(B2,1,4)," ",MID(C2,1,3)," ",MID(D2,1,3)," Grp.",F2)</f>
-        <v>MATE DISC   Grp.W</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+        <f>CONCATENATE(MID(A2,1,4)," ",MID(B2,1,4)," ",MID(C2,1,3)," ",MID(D2,1,3)," Grp.",F2)</f>
+        <v>INIC DISC   Grp.W</v>
+      </c>
+      <c r="J2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="8"/>
       <c r="D3" s="9"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="G3" s="8">
         <v>1</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I3" s="13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I3:I39" si="0">CONCATENATE(MID(A3,1,4)," ",MID(B3,1,4)," ",MID(C3,1,3)," ",MID(D3,1,3)," Grp.",F3)</f>
         <v>MATE DISC   Grp.W1</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="G4" s="8">
         <v>1</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I4" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FUND CIEN COM  Grp.M</v>
       </c>
       <c r="J4" s="13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="K4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="e">
         <v>#REF!</v>
       </c>
@@ -1513,139 +1523,139 @@
       <c r="D5" s="9"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="G5" s="8">
         <v>1</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I5" s="13" t="e">
         <f t="shared" si="0"/>
         <v>#REF!</v>
       </c>
-      <c r="J5" s="13" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J5" s="13" t="e">
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="8">
         <v>1</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I6" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ADMI PROG BAS DAT Grp.C</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="9"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
       <c r="G7" s="8">
         <v>1</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I7" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INTR INFO   Grp.1M</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G8" s="8">
         <v>1</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I8" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INFO APLI TEC  Grp.C</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G9" s="8">
         <v>1</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I9" s="13" t="str">
         <f t="shared" si="0"/>
         <v>PROG LÓGI FUN  Grp.A</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -1662,284 +1672,284 @@
         <v>19</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="G10" s="8">
         <v>1</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I10" s="13" t="str">
         <f t="shared" si="0"/>
         <v>PROY INTE DES SOL Grp.S1</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="9"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="G11" s="8">
         <v>1</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I11" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INTR INFO   Grp.2M</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="G12" s="8">
         <v>1</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I12" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INFO APLI TEC  Grp.F</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G13" s="8">
         <v>1</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I13" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ORGA ARQU COM  Grp.A</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G14" s="8">
         <v>1</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I14" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ADMI SIST OPE  Grp.A</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E15" s="8"/>
       <c r="F15" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="G15" s="8">
         <v>1</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I15" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INFR TI TEC EME Grp.S1</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="9"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G16" s="8">
         <v>1</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I16" s="13" t="str">
         <f t="shared" si="0"/>
         <v>COMU I   Grp.A</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G17" s="8">
         <v>1</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I17" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FUND COMU   Grp.A</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G18" s="8">
         <v>1</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I18" s="13" t="str">
         <f t="shared" si="0"/>
         <v>TEOR COMU   Grp.C</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="G19" s="8">
         <v>1</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I19" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INTR INFO   Grp.F</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="8"/>
@@ -1950,14 +1960,14 @@
         <v>1</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I20" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INTR INFO SEM  Grp.B</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -1965,111 +1975,111 @@
         <v>15</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="9"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G21" s="8">
         <v>1</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I21" s="13" t="str">
         <f t="shared" si="0"/>
         <v>PROY EMPR   Grp.11</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="9"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G22" s="8">
         <v>1</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I22" s="13" t="str">
         <f t="shared" si="0"/>
         <v>MATE DISC   Grp.L</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="8" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G23" s="8">
         <v>1</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I23" s="13" t="str">
         <f t="shared" si="0"/>
         <v>FUND CIEN COM  Grp.J</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="8"/>
       <c r="F24" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G24" s="8">
         <v>1</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I24" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INFO APLI TEC  Grp.E</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2077,7 +2087,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="8"/>
@@ -2089,161 +2099,161 @@
         <v>1</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I25" s="13" t="str">
         <f t="shared" si="0"/>
         <v>TALL PROG   Grp.B</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="8"/>
       <c r="F26" s="8" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="G26" s="8">
         <v>1</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I26" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ORGA ARQU COM  Grp.S1</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G27" s="8">
         <v>1</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I27" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ADMI SIST OPE  Grp.SN</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="E28" s="8"/>
       <c r="F28" s="8" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="G28" s="8">
         <v>1</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I28" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INFR TI TEC EME Grp.SN</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
       <c r="F29" s="8" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G29" s="8">
         <v>1</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I29" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ANTE SIST RAD  Grp.R1</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
       <c r="F30" s="8" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="G30" s="8">
         <v>1</v>
       </c>
       <c r="H30" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I30" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ANTE SIST RAD  Grp.R1</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2251,26 +2261,26 @@
         <v>20</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G31" s="8">
         <v>1</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I31" s="13" t="str">
         <f t="shared" si="0"/>
         <v>TALL REDE   Grp.RN</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2278,169 +2288,169 @@
         <v>12</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8"/>
       <c r="F32" s="8" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="G32" s="8">
         <v>1</v>
       </c>
       <c r="H32" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I32" s="13" t="str">
         <f t="shared" si="0"/>
         <v>DISE CABL EST  Grp.R2</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
       <c r="F33" s="8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G33" s="8">
         <v>1</v>
       </c>
       <c r="H33" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I33" s="13" t="str">
         <f t="shared" si="0"/>
         <v>CABL ESTR   Grp.RN</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
-        <v>101</v>
+        <v>59</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
       <c r="F34" s="8" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G34" s="8">
         <v>1</v>
       </c>
       <c r="H34" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I34" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INST REDE   Grp.H</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
       <c r="F35" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G35" s="8">
         <v>1</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I35" s="13" t="str">
         <f t="shared" si="0"/>
         <v>INTR INFO SEM  Grp.C</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="9"/>
       <c r="E36" s="8"/>
       <c r="F36" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="G36" s="8">
         <v>1</v>
       </c>
       <c r="H36" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I36" s="13" t="str">
         <f t="shared" si="0"/>
         <v>PROG III   Grp.TU</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="E37" s="8"/>
       <c r="F37" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="G37" s="8">
         <v>1</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I37" s="13" t="str">
         <f t="shared" si="0"/>
         <v>ADMI SIST OPE VI Grp.TU</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
@@ -2448,64 +2458,66 @@
         <v>17</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>110</v>
+        <v>62</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>108</v>
+        <v>61</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="G38" s="8">
         <v>1</v>
       </c>
       <c r="H38" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I38" s="13" t="str">
         <f t="shared" si="0"/>
         <v>DESA APLI VI  Grp.TU</v>
       </c>
       <c r="J38" s="13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="8"/>
       <c r="F39" s="8" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="G39" s="8">
         <v>1</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I39" s="13" t="str">
         <f t="shared" si="0"/>
         <v>COMP PARA DIS  Grp.TU</v>
       </c>
       <c r="J39" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>